<commit_message>
RD Major Flow Changes
</commit_message>
<xml_diff>
--- a/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
+++ b/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+  <si>
+    <t>Mobile_Number</t>
+  </si>
   <si>
     <t>Pincode</t>
   </si>
@@ -32,9 +35,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Mobile_Number</t>
-  </si>
-  <si>
     <t>OTP1</t>
   </si>
   <si>
@@ -62,6 +62,87 @@
     <t>Last_name</t>
   </si>
   <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Investment amount</t>
+  </si>
+  <si>
+    <t>Tenure</t>
+  </si>
+  <si>
+    <t>Installment_date</t>
+  </si>
+  <si>
+    <t>Doc_type</t>
+  </si>
+  <si>
+    <t>Doc_num</t>
+  </si>
+  <si>
+    <t>Proof_front</t>
+  </si>
+  <si>
+    <t>Proof_back</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Photo_upload</t>
+  </si>
+  <si>
+    <t>Account_number</t>
+  </si>
+  <si>
+    <t>Confirm_acc_number</t>
+  </si>
+  <si>
+    <t>IFSC</t>
+  </si>
+  <si>
+    <t>Acc_name</t>
+  </si>
+  <si>
+    <t>Cheque_upload</t>
+  </si>
+  <si>
+    <t>Maturity_instruction</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Father_name</t>
+  </si>
+  <si>
+    <t>Marital_status</t>
+  </si>
+  <si>
+    <t>Fd_tenure</t>
+  </si>
+  <si>
+    <t>FD_payout</t>
+  </si>
+  <si>
+    <t>Nom_relationship</t>
+  </si>
+  <si>
+    <t>Nom_title</t>
+  </si>
+  <si>
+    <t>Nom_first_name</t>
+  </si>
+  <si>
+    <t>Nom_last_name</t>
+  </si>
+  <si>
     <t>CMMPD4348G</t>
   </si>
   <si>
@@ -71,99 +152,27 @@
     <t>sekar</t>
   </si>
   <si>
-    <t>Mail</t>
-  </si>
-  <si>
     <t>dillibai@novactech.in</t>
   </si>
   <si>
-    <t>Investment amount</t>
-  </si>
-  <si>
-    <t>Tenure</t>
-  </si>
-  <si>
-    <t>Installment_date</t>
-  </si>
-  <si>
-    <t>Doc_type</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aadhaar ID</t>
   </si>
   <si>
-    <t>Doc_num</t>
-  </si>
-  <si>
-    <t>Proof_front</t>
-  </si>
-  <si>
-    <t>Proof_back</t>
-  </si>
-  <si>
     <t>E:\Python Project\Python\PycharmProject\pythonProject1\InputFiles\GoldLoan.jpeg</t>
   </si>
   <si>
-    <t>Address2</t>
-  </si>
-  <si>
-    <t>Address1</t>
-  </si>
-  <si>
-    <t>Photo_upload</t>
+    <t>No.16/6</t>
   </si>
   <si>
     <t>Gangai amman kovil 1st street</t>
   </si>
   <si>
-    <t>No.16/6</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t xml:space="preserve">ETHIRAJ SALAI, CHENNAI, TAMIL NADU, 600008 </t>
   </si>
   <si>
-    <t>Account_number</t>
-  </si>
-  <si>
-    <t>Confirm_acc_number</t>
-  </si>
-  <si>
-    <t>Acc_name</t>
-  </si>
-  <si>
-    <t>IFSC</t>
-  </si>
-  <si>
     <t>HDFC0001297</t>
   </si>
   <si>
-    <t>Cheque_upload</t>
-  </si>
-  <si>
-    <t>111111111111111111</t>
-  </si>
-  <si>
-    <t>777755553214</t>
-  </si>
-  <si>
-    <t>Maturity_instruction</t>
-  </si>
-  <si>
-    <t>Occupation</t>
-  </si>
-  <si>
-    <t>Marital_status</t>
-  </si>
-  <si>
-    <t>Fd_tenure</t>
-  </si>
-  <si>
-    <t>FD_payout</t>
-  </si>
-  <si>
     <t>RDCFD</t>
   </si>
   <si>
@@ -179,18 +188,6 @@
     <t>QTR</t>
   </si>
   <si>
-    <t>Nom_relationship</t>
-  </si>
-  <si>
-    <t>Nom_title</t>
-  </si>
-  <si>
-    <t>Nom_first_name</t>
-  </si>
-  <si>
-    <t>Nom_last_name</t>
-  </si>
-  <si>
     <t>FATHR</t>
   </si>
   <si>
@@ -200,57 +197,23 @@
     <t>Ramasamy</t>
   </si>
   <si>
-    <t>6777890098</t>
-  </si>
-  <si>
-    <t>Father_name</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>6777890091</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>9988887799</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF54B33E"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,32 +233,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,49 +519,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN10"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" style="1" customWidth="1"/>
-    <col min="19" max="22" width="9.140625" style="1"/>
-    <col min="23" max="23" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="6"/>
-    <col min="25" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="18.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="45">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -646,259 +569,214 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>54</v>
-      </c>
     </row>
-    <row r="2" spans="1:40" ht="165">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1">
         <v>600026</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>61</v>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="N2" s="1">
         <v>500</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="1">
         <v>36</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="1">
         <v>25</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="R2" s="1">
+        <v>777755553214</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="W2" s="1">
         <v>600026</v>
       </c>
-      <c r="X2" s="5" t="s">
-        <v>32</v>
+      <c r="X2" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1.1111111111111101E+17</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1.1111111111111101E+17</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" s="7">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI2" s="1">
         <v>36</v>
       </c>
-      <c r="AJ2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AJ2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AM2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:40">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:40">
-      <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40">
-      <c r="A8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40">
-      <c r="A9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40">
-      <c r="A10" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
driver-wait untill ele visible
</commit_message>
<xml_diff>
--- a/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
+++ b/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Mobile_Number</t>
   </si>
@@ -201,19 +201,42 @@
   </si>
   <si>
     <t>9988877799</t>
+  </si>
+  <si>
+    <t>Nom_ad1</t>
+  </si>
+  <si>
+    <t>Vadapalani</t>
+  </si>
+  <si>
+    <t>Nom_ad2</t>
+  </si>
+  <si>
+    <t>Gangai amman kovil street</t>
+  </si>
+  <si>
+    <t>Nom_pincode</t>
+  </si>
+  <si>
+    <t>777755553214</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,9 +259,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,19 +545,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,8 +678,17 @@
       <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="AO1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -705,8 +740,8 @@
       <c r="Q2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1">
-        <v>777755553214</v>
+      <c r="R2" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>44</v>
@@ -773,6 +808,15 @@
       </c>
       <c r="AN2" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>600026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sendkeys changes and OS path fetch
</commit_message>
<xml_diff>
--- a/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
+++ b/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
@@ -158,9 +158,6 @@
     <t xml:space="preserve"> Aadhaar ID</t>
   </si>
   <si>
-    <t>E:\Python Project\Python\PycharmProject\pythonProject1\InputFiles\GoldLoan.jpeg</t>
-  </si>
-  <si>
     <t>No.16/6</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>9988877799</t>
-  </si>
-  <si>
     <t>Nom_ad1</t>
   </si>
   <si>
@@ -219,6 +213,12 @@
   </si>
   <si>
     <t>777755553214</t>
+  </si>
+  <si>
+    <t>9988899999</t>
+  </si>
+  <si>
+    <t>InputFiles\GoldLoan.jpeg</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,24 +679,24 @@
         <v>38</v>
       </c>
       <c r="AO1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1">
         <v>600026</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -741,28 +741,28 @@
         <v>43</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="W2" s="1">
         <v>600026</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="Z2" s="1">
         <v>1.1111111111111101E+17</v>
@@ -771,49 +771,49 @@
         <v>1.1111111111111101E+17</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="AE2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="AI2" s="1">
         <v>36</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="AO2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AQ2" s="1">
         <v>600026</v>

</xml_diff>

<commit_message>
changes in drop-down func
</commit_message>
<xml_diff>
--- a/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
+++ b/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
@@ -170,9 +170,6 @@
     <t>HDFC0001297</t>
   </si>
   <si>
-    <t>RDCFD</t>
-  </si>
-  <si>
     <t>PROFL</t>
   </si>
   <si>
@@ -215,17 +212,20 @@
     <t>777755553214</t>
   </si>
   <si>
-    <t>9988899999</t>
-  </si>
-  <si>
     <t>InputFiles\GoldLoan.jpeg</t>
+  </si>
+  <si>
+    <t>7708273167</t>
+  </si>
+  <si>
+    <t>RDROM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +237,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,12 +265,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,13 +686,13 @@
         <v>38</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:43">
@@ -696,7 +703,7 @@
         <v>600026</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -741,13 +748,13 @@
         <v>43</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>44</v>
@@ -762,7 +769,7 @@
         <v>46</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z2" s="1">
         <v>1.1111111111111101E+17</v>
@@ -777,43 +784,43 @@
         <v>40</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="AI2" s="1">
         <v>36</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="AO2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AQ2" s="1">
         <v>600026</v>

</xml_diff>

<commit_message>
Fetch FD article URLs by tag name'table'
</commit_message>
<xml_diff>
--- a/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
+++ b/PycharmProject/pythonProject1/InputFiles/RD_DATA.xlsx
@@ -215,10 +215,10 @@
     <t>InputFiles\GoldLoan.jpeg</t>
   </si>
   <si>
-    <t>7708273167</t>
-  </si>
-  <si>
     <t>RDROM</t>
+  </si>
+  <si>
+    <t>7709856398</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,7 +697,7 @@
     </row>
     <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1">
         <v>600026</v>
@@ -787,7 +787,7 @@
         <v>62</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>48</v>

</xml_diff>